<commit_message>
Correcciones añadidas a los archivos
</commit_message>
<xml_diff>
--- a/CARACT PEP.xlsx
+++ b/CARACT PEP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javeb\Desktop\GITHUB\TareaR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199FB866-F33F-49F7-9503-5BB64ABC8912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F084D29-0815-4731-92B5-D281148865A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="160">
   <si>
     <t>nombre</t>
   </si>
@@ -435,9 +435,6 @@
   </si>
   <si>
     <t>ID en uniprot</t>
-  </si>
-  <si>
-    <t>digestion realizada en BIOPEP</t>
   </si>
   <si>
     <t>https://biochemia.uwm.edu.pl/en/biopep-uwm-2/</t>
@@ -491,6 +488,52 @@
   </si>
   <si>
     <t xml:space="preserve">Compute the FASGAI vectors </t>
+  </si>
+  <si>
+    <t>The FASGAI vectors (Factor Analysis Scales of Generalized Amino Acid Information) is a set of
+amino acid descriptors, that reflects hydrophobicity, alpha and turn propensities, bulky properties,
+compositional characteristics, local flexibility, and electronic properties, that can be utilized to rep resent the sequence structural features of peptides or protein motifs.</t>
+  </si>
+  <si>
+    <t>Electronic properties</t>
+  </si>
+  <si>
+    <t>Local flexibility,</t>
+  </si>
+  <si>
+    <t>Compositional characteristic index,</t>
+  </si>
+  <si>
+    <t>Bulky properties,</t>
+  </si>
+  <si>
+    <t>Alpha and turn propensities,</t>
+  </si>
+  <si>
+    <t>Hydrophobicity index,</t>
+  </si>
+  <si>
+    <t>This function calculates the GRAVY hydrophobicity index of an amino acids sequence using one
+of the 38 scales from different sources.</t>
+  </si>
+  <si>
+    <t>The isoelectric point (pI), is the pH at which a particular molecule or surface carries no net electrical
+charge.</t>
+  </si>
+  <si>
+    <t>HIDROPHOBICITY</t>
+  </si>
+  <si>
+    <t>ISOELECTRIC POINT</t>
+  </si>
+  <si>
+    <t>NET CHARGE</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/</t>
+  </si>
+  <si>
+    <t>digestion realizada en BIOPEP con subtilisina</t>
   </si>
 </sst>
 </file>
@@ -658,7 +701,7 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -674,16 +717,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -914,13 +947,13 @@
   <dimension ref="A1:O1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.54296875" customWidth="1"/>
     <col min="5" max="5" width="20.81640625" customWidth="1"/>
     <col min="6" max="6" width="75.453125" customWidth="1"/>
@@ -1195,8 +1228,16 @@
     <row r="12" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C12" s="15"/>
     </row>
-    <row r="13" spans="1:15" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="C13" s="15"/>
+    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
@@ -1205,17 +1246,19 @@
       <c r="B14" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>132</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
@@ -1223,7 +1266,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C16" s="15"/>
     </row>
@@ -1232,7 +1275,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="15"/>
     </row>
@@ -1241,7 +1284,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="15"/>
     </row>
@@ -1250,16 +1293,16 @@
         <v>44</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>141</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>142</v>
       </c>
       <c r="C20" s="15"/>
     </row>
@@ -1268,7 +1311,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="15"/>
     </row>
@@ -1277,7 +1320,7 @@
         <v>46</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" s="15"/>
     </row>
@@ -1286,83 +1329,101 @@
         <v>47</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:3" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B24" s="23"/>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>48</v>
       </c>
+      <c r="B25" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="C25" s="15"/>
     </row>
     <row r="26" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>49</v>
       </c>
+      <c r="B26" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>50</v>
       </c>
+      <c r="B27" s="23" t="s">
+        <v>150</v>
+      </c>
       <c r="C27" s="15"/>
     </row>
     <row r="28" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>51</v>
       </c>
+      <c r="B28" s="23" t="s">
+        <v>149</v>
+      </c>
       <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>52</v>
       </c>
+      <c r="B29" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="C29" s="15"/>
     </row>
     <row r="30" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="B30" s="23" t="s">
+        <v>147</v>
+      </c>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>54</v>
       </c>
+      <c r="B31" s="25" t="s">
+        <v>153</v>
+      </c>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>55</v>
       </c>
+      <c r="B32" s="25" t="s">
+        <v>153</v>
+      </c>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>56</v>
       </c>
+      <c r="B33" s="25" t="s">
+        <v>154</v>
+      </c>
       <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="35" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C35" s="15"/>
@@ -4298,8 +4359,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4330,7 +4391,7 @@
         <v>43</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>45</v>
@@ -4360,13 +4421,13 @@
         <v>53</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="16" t="s">
         <v>55</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="S1" s="18"/>
       <c r="T1" s="18"/>
@@ -9858,7 +9919,7 @@
         <v>115</v>
       </c>
       <c r="C98" s="20" t="str">
-        <f t="shared" ref="C98:C129" si="3">IF(COUNTIF(B:B,B98)&gt;1,"DUPLICATE", "UNIQUE")</f>
+        <f t="shared" ref="C98:C109" si="3">IF(COUNTIF(B:B,B98)&gt;1,"DUPLICATE", "UNIQUE")</f>
         <v>DUPLICATE</v>
       </c>
       <c r="D98" s="22">

</xml_diff>